<commit_message>
querys: vendas por categoria, compras acima da média
</commit_message>
<xml_diff>
--- a/dados/ETL FISICA/NextplayFisica.xlsx
+++ b/dados/ETL FISICA/NextplayFisica.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Daniel\Desktop\Dados_NEXTPLAY\ETL FISICA\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Daniel\Desktop\NextPlay\dados\ETL FISICA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F009CAF9-28F0-4666-9621-DBE77B0931B9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D266BD83-C6D4-491E-9FE2-7A28BD376F54}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="2" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="categorias" sheetId="2" r:id="rId1"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="513" uniqueCount="307">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="501" uniqueCount="306">
   <si>
     <t>PLAYSTATION 5 1 CONTROLE</t>
   </si>
@@ -945,9 +945,6 @@
   </si>
   <si>
     <t>DINHEIRO</t>
-  </si>
-  <si>
-    <t>DEBITO</t>
   </si>
   <si>
     <t>ID_ITEM_VENDA</t>
@@ -969,11 +966,12 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="2">
+  <numFmts count="3">
+    <numFmt numFmtId="8" formatCode="&quot;R$&quot;\ #,##0.00;[Red]\-&quot;R$&quot;\ #,##0.00"/>
     <numFmt numFmtId="44" formatCode="_-&quot;R$&quot;\ * #,##0.00_-;\-&quot;R$&quot;\ * #,##0.00_-;_-&quot;R$&quot;\ * &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="164" formatCode="_-[$R$-416]\ * #,##0.00_-;\-[$R$-416]\ * #,##0.00_-;_-[$R$-416]\ * &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
-  <fonts count="11" x14ac:knownFonts="1">
+  <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1051,10 +1049,17 @@
     <font>
       <sz val="10"/>
       <color theme="1"/>
-      <name val="MonTSERRAT"/>
+      <name val="Montserrat"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1085,8 +1090,14 @@
         <bgColor theme="5"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFD9D9D9"/>
+        <bgColor rgb="FFD9D9D9"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="11">
+  <borders count="14">
     <border>
       <left/>
       <right/>
@@ -1218,13 +1229,40 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="44" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="57">
+  <cellXfs count="70">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1320,16 +1358,6 @@
     <xf numFmtId="14" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1384,13 +1412,62 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="8" fontId="11" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="11" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="6" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="8" fontId="11" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="11" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="6" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="8" fontId="11" fillId="6" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="6" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="11" fillId="6" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Hiperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Moeda" xfId="2" builtinId="4"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="76">
+  <dxfs count="74">
     <dxf>
       <font>
         <strike val="0"/>
@@ -1398,12 +1475,24 @@
         <shadow val="0"/>
         <u val="none"/>
         <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color theme="1"/>
-        <name val="MonTSERRAT"/>
-        <scheme val="none"/>
+        <sz val="11"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
       </font>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
       <border diagonalUp="0" diagonalDown="0" outline="0">
         <left style="thin">
           <color indexed="64"/>
@@ -1411,29 +1500,8 @@
         <right style="thin">
           <color indexed="64"/>
         </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
+        <top/>
+        <bottom/>
       </border>
     </dxf>
     <dxf>
@@ -1443,61 +1511,63 @@
         <shadow val="0"/>
         <u val="none"/>
         <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color theme="1"/>
-        <name val="MonTSERRAT"/>
-        <scheme val="none"/>
+        <sz val="11"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
       </font>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left/>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
     </dxf>
     <dxf>
       <font>
-        <color rgb="FF9C0006"/>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
       </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
     </dxf>
     <dxf>
       <font>
-        <color rgb="FF9C5700"/>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
       </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
     </dxf>
     <dxf>
       <font>
@@ -1563,6 +1633,94 @@
         </bottom>
         <vertical/>
         <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <name val="MonTSERRAT"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <name val="MonTSERRAT"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
       </border>
     </dxf>
     <dxf>
@@ -2119,87 +2277,6 @@
       </border>
     </dxf>
     <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right/>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left/>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
       <border>
         <top style="thin">
           <color indexed="64"/>
@@ -2223,31 +2300,10 @@
       </border>
     </dxf>
     <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
       <border>
         <bottom style="thin">
           <color indexed="64"/>
         </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top/>
-        <bottom/>
-        <vertical style="thin">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
       </border>
     </dxf>
     <dxf>
@@ -2652,102 +2708,102 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{4844B637-AF78-489F-AE84-54145DD12A14}" name="Tabela6" displayName="Tabela6" ref="A1:B19" totalsRowShown="0" headerRowDxfId="75" dataDxfId="73" headerRowBorderDxfId="74" tableBorderDxfId="72" totalsRowBorderDxfId="71">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{4844B637-AF78-489F-AE84-54145DD12A14}" name="Tabela6" displayName="Tabela6" ref="A1:B19" totalsRowShown="0" headerRowDxfId="73" dataDxfId="71" headerRowBorderDxfId="72" tableBorderDxfId="70" totalsRowBorderDxfId="69">
   <autoFilter ref="A1:B19" xr:uid="{4844B637-AF78-489F-AE84-54145DD12A14}"/>
   <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{EC223AE9-F9A0-497B-A3D0-F6DBA2FA3827}" name="ID_CATEGORIA" dataDxfId="70"/>
-    <tableColumn id="2" xr3:uid="{7C9D6326-6E35-4B14-9C54-F6C5259FC899}" name="CATEGORIA" dataDxfId="69"/>
+    <tableColumn id="1" xr3:uid="{EC223AE9-F9A0-497B-A3D0-F6DBA2FA3827}" name="ID_CATEGORIA" dataDxfId="68"/>
+    <tableColumn id="2" xr3:uid="{7C9D6326-6E35-4B14-9C54-F6C5259FC899}" name="CATEGORIA" dataDxfId="67"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium17" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{85BD5BEE-FE84-4B60-99A0-A2F85BCD1D1F}" name="Tabela2" displayName="Tabela2" ref="A1:F100" totalsRowShown="0" headerRowDxfId="68" dataDxfId="66" headerRowBorderDxfId="67" tableBorderDxfId="65">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{85BD5BEE-FE84-4B60-99A0-A2F85BCD1D1F}" name="Tabela2" displayName="Tabela2" ref="A1:F100" totalsRowShown="0" headerRowDxfId="66" dataDxfId="64" headerRowBorderDxfId="65" tableBorderDxfId="63">
   <autoFilter ref="A1:F100" xr:uid="{85BD5BEE-FE84-4B60-99A0-A2F85BCD1D1F}"/>
   <tableColumns count="6">
-    <tableColumn id="1" xr3:uid="{CAF43EEC-408C-408D-BB00-A3EB8F300051}" name="ID_CLIENTE" dataDxfId="64"/>
-    <tableColumn id="2" xr3:uid="{C2B7634E-2753-42D2-BA3C-61EA5EA45B60}" name="NOME" dataDxfId="63"/>
-    <tableColumn id="3" xr3:uid="{FAF28948-E94B-4D8D-B94F-CBA52D50F4D8}" name="TELEFONE" dataDxfId="62"/>
-    <tableColumn id="4" xr3:uid="{68075F99-35E7-49C5-A9CB-C40DB0B4883C}" name="EMAIL" dataDxfId="61"/>
-    <tableColumn id="6" xr3:uid="{46A5DC73-2FAA-418A-B466-898C9590D123}" name="ID_ENDERECO" dataDxfId="60"/>
-    <tableColumn id="7" xr3:uid="{4FA5C767-F544-45DB-9AC2-1097B66AD58C}" name="SEXO" dataDxfId="59"/>
+    <tableColumn id="1" xr3:uid="{CAF43EEC-408C-408D-BB00-A3EB8F300051}" name="ID_CLIENTE" dataDxfId="62"/>
+    <tableColumn id="2" xr3:uid="{C2B7634E-2753-42D2-BA3C-61EA5EA45B60}" name="NOME" dataDxfId="61"/>
+    <tableColumn id="3" xr3:uid="{FAF28948-E94B-4D8D-B94F-CBA52D50F4D8}" name="TELEFONE" dataDxfId="60"/>
+    <tableColumn id="4" xr3:uid="{68075F99-35E7-49C5-A9CB-C40DB0B4883C}" name="EMAIL" dataDxfId="59"/>
+    <tableColumn id="6" xr3:uid="{46A5DC73-2FAA-418A-B466-898C9590D123}" name="ID_ENDERECO" dataDxfId="58"/>
+    <tableColumn id="7" xr3:uid="{4FA5C767-F544-45DB-9AC2-1097B66AD58C}" name="SEXO" dataDxfId="57"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{03B2F8B8-4423-439D-870B-A087290BC89F}" name="Tabela5" displayName="Tabela5" ref="A1:E21" totalsRowShown="0" headerRowDxfId="58" dataDxfId="56" headerRowBorderDxfId="57" tableBorderDxfId="55" totalsRowBorderDxfId="54">
-  <autoFilter ref="A1:E21" xr:uid="{03B2F8B8-4423-439D-870B-A087290BC89F}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{03B2F8B8-4423-439D-870B-A087290BC89F}" name="Tabela5" displayName="Tabela5" ref="A1:E9" totalsRowShown="0" headerRowDxfId="1" dataDxfId="0" headerRowBorderDxfId="56" tableBorderDxfId="55" totalsRowBorderDxfId="54">
+  <autoFilter ref="A1:E9" xr:uid="{03B2F8B8-4423-439D-870B-A087290BC89F}"/>
   <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{5D27014E-A127-4501-835C-98E52838FCBC}" name="ID_VENDAS" dataDxfId="53"/>
-    <tableColumn id="2" xr3:uid="{754703C4-E233-497C-AD1E-EDE5CA73B6C2}" name="VALOR_TOTAL" dataDxfId="52"/>
-    <tableColumn id="3" xr3:uid="{BB454188-8C4E-4EEE-A281-86D37A24E086}" name="METODO_PAGAMENTO" dataDxfId="51"/>
-    <tableColumn id="4" xr3:uid="{1CD8B93A-294F-47BD-BFE3-42218BE0813B}" name="DATA_VENDA" dataDxfId="50"/>
-    <tableColumn id="5" xr3:uid="{599A70D0-83B4-4506-B9E2-76E0C3FDBB62}" name="ID_CLIENTE" dataDxfId="49"/>
+    <tableColumn id="1" xr3:uid="{5D27014E-A127-4501-835C-98E52838FCBC}" name="ID_VENDAS" dataDxfId="6"/>
+    <tableColumn id="2" xr3:uid="{754703C4-E233-497C-AD1E-EDE5CA73B6C2}" name="VALOR_TOTAL" dataDxfId="5"/>
+    <tableColumn id="3" xr3:uid="{BB454188-8C4E-4EEE-A281-86D37A24E086}" name="METODO_PAGAMENTO" dataDxfId="4"/>
+    <tableColumn id="4" xr3:uid="{1CD8B93A-294F-47BD-BFE3-42218BE0813B}" name="DATA_VENDA" dataDxfId="3"/>
+    <tableColumn id="5" xr3:uid="{599A70D0-83B4-4506-B9E2-76E0C3FDBB62}" name="ID_CLIENTE" dataDxfId="2"/>
   </tableColumns>
-  <tableStyleInfo name="TableStyleMedium17" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+  <tableStyleInfo name="TableStyleLight10" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{A73D557B-39B5-452D-A79E-8AAC86A6488D}" name="Tabela4" displayName="Tabela4" ref="A1:E31" totalsRowShown="0" headerRowDxfId="48" dataDxfId="46" headerRowBorderDxfId="47" tableBorderDxfId="45" totalsRowBorderDxfId="44">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{A73D557B-39B5-452D-A79E-8AAC86A6488D}" name="Tabela4" displayName="Tabela4" ref="A1:E31" totalsRowShown="0" headerRowDxfId="53" dataDxfId="51" headerRowBorderDxfId="52" tableBorderDxfId="50" totalsRowBorderDxfId="49">
   <autoFilter ref="A1:E31" xr:uid="{A73D557B-39B5-452D-A79E-8AAC86A6488D}"/>
   <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{CAFC33D8-DDEC-41FB-94FC-49F0148A57AE}" name="ID_ITEM_VENDA" dataDxfId="43"/>
-    <tableColumn id="2" xr3:uid="{E2BE1EB4-69BB-46EB-B145-5EE83D0A75E3}" name="ID_VENDA" dataDxfId="42"/>
-    <tableColumn id="3" xr3:uid="{AC1C0DC3-98B6-4C51-9537-497B08BC3640}" name="ID_PRODUTO" dataDxfId="41"/>
-    <tableColumn id="4" xr3:uid="{9BA9E6C7-7143-4BDB-8F6D-001FC42184FC}" name="QUANTIDADE" dataDxfId="40"/>
-    <tableColumn id="5" xr3:uid="{2B9B9B7D-C418-4AB0-A880-EA2386FFA980}" name="PRECO_UNITARIO" dataDxfId="39"/>
+    <tableColumn id="1" xr3:uid="{CAFC33D8-DDEC-41FB-94FC-49F0148A57AE}" name="ID_ITEM_VENDA" dataDxfId="48"/>
+    <tableColumn id="2" xr3:uid="{E2BE1EB4-69BB-46EB-B145-5EE83D0A75E3}" name="ID_VENDA" dataDxfId="47"/>
+    <tableColumn id="3" xr3:uid="{AC1C0DC3-98B6-4C51-9537-497B08BC3640}" name="ID_PRODUTO" dataDxfId="46"/>
+    <tableColumn id="4" xr3:uid="{9BA9E6C7-7143-4BDB-8F6D-001FC42184FC}" name="QUANTIDADE" dataDxfId="45"/>
+    <tableColumn id="5" xr3:uid="{2B9B9B7D-C418-4AB0-A880-EA2386FFA980}" name="PRECO_UNITARIO" dataDxfId="44"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium17" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{B4E5282A-C5FE-47C6-A157-F22D4207A94C}" name="Tabela1" displayName="Tabela1" ref="A1:F38" totalsRowCount="1" headerRowDxfId="38" dataDxfId="36" headerRowBorderDxfId="37" tableBorderDxfId="35" totalsRowBorderDxfId="34">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{B4E5282A-C5FE-47C6-A157-F22D4207A94C}" name="Tabela1" displayName="Tabela1" ref="A1:F38" totalsRowCount="1" headerRowDxfId="43" dataDxfId="41" headerRowBorderDxfId="42" tableBorderDxfId="40" totalsRowBorderDxfId="39">
   <autoFilter ref="A1:F37" xr:uid="{B4E5282A-C5FE-47C6-A157-F22D4207A94C}"/>
   <tableColumns count="6">
-    <tableColumn id="1" xr3:uid="{12BDCA2A-5D80-474D-B2F4-DB327E4455C1}" name="ID_PRODUTO" dataDxfId="33" totalsRowDxfId="32"/>
-    <tableColumn id="2" xr3:uid="{B797EDEC-5E65-4533-8484-4897511B1C7F}" name="NOME" dataDxfId="31" totalsRowDxfId="30"/>
-    <tableColumn id="3" xr3:uid="{BD03FBB8-BAFB-4686-B914-6ECADC3030C4}" name="DESCRICAO" dataDxfId="29" totalsRowDxfId="28"/>
-    <tableColumn id="4" xr3:uid="{2381DBFB-717C-4AF6-8C40-7B7F3BB975BB}" name="PRECO" dataDxfId="27" totalsRowDxfId="26"/>
-    <tableColumn id="5" xr3:uid="{D7A17B66-93A5-454D-A407-445C48DB1F6C}" name="QTD_ESTOQUE" totalsRowFunction="custom" dataDxfId="25" totalsRowDxfId="24">
+    <tableColumn id="1" xr3:uid="{12BDCA2A-5D80-474D-B2F4-DB327E4455C1}" name="ID_PRODUTO" dataDxfId="38" totalsRowDxfId="37"/>
+    <tableColumn id="2" xr3:uid="{B797EDEC-5E65-4533-8484-4897511B1C7F}" name="NOME" dataDxfId="36" totalsRowDxfId="35"/>
+    <tableColumn id="3" xr3:uid="{BD03FBB8-BAFB-4686-B914-6ECADC3030C4}" name="DESCRICAO" dataDxfId="34" totalsRowDxfId="33"/>
+    <tableColumn id="4" xr3:uid="{2381DBFB-717C-4AF6-8C40-7B7F3BB975BB}" name="PRECO" dataDxfId="32" totalsRowDxfId="31"/>
+    <tableColumn id="5" xr3:uid="{D7A17B66-93A5-454D-A407-445C48DB1F6C}" name="QTD_ESTOQUE" totalsRowFunction="custom" dataDxfId="30" totalsRowDxfId="29">
       <totalsRowFormula>SUM(Tabela1[QTD_ESTOQUE])</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{E846FE5F-32B4-46A1-81E2-005277F0615B}" name="ID_CATEGORIA" dataDxfId="23" totalsRowDxfId="22"/>
+    <tableColumn id="6" xr3:uid="{E846FE5F-32B4-46A1-81E2-005277F0615B}" name="ID_CATEGORIA" dataDxfId="28" totalsRowDxfId="27"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium17" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{E2441FD0-F666-49F4-810E-B81BBCB31B65}" name="Tabela3" displayName="Tabela3" ref="A1:D2" totalsRowShown="0" headerRowDxfId="21" dataDxfId="20">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{E2441FD0-F666-49F4-810E-B81BBCB31B65}" name="Tabela3" displayName="Tabela3" ref="A1:D2" totalsRowShown="0" headerRowDxfId="26" dataDxfId="25">
   <autoFilter ref="A1:D2" xr:uid="{E2441FD0-F666-49F4-810E-B81BBCB31B65}"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{6FAE7983-2A81-4BDA-A59F-AA6C4E6F190C}" name="ID_GASTOS" dataDxfId="19"/>
-    <tableColumn id="2" xr3:uid="{4C238707-ADEB-44AE-A33F-11E670FC3464}" name="SALARIOS" dataDxfId="18"/>
-    <tableColumn id="3" xr3:uid="{DD3A0721-15BF-48D5-83F5-250B9BA824CE}" name="COMPRA_ESTOQUE" dataDxfId="17"/>
-    <tableColumn id="4" xr3:uid="{DA9386F6-AAE0-4E57-903A-B2F98B6704B9}" name="DATA" dataDxfId="16"/>
+    <tableColumn id="1" xr3:uid="{6FAE7983-2A81-4BDA-A59F-AA6C4E6F190C}" name="ID_GASTOS" dataDxfId="24"/>
+    <tableColumn id="2" xr3:uid="{4C238707-ADEB-44AE-A33F-11E670FC3464}" name="SALARIOS" dataDxfId="23"/>
+    <tableColumn id="3" xr3:uid="{DD3A0721-15BF-48D5-83F5-250B9BA824CE}" name="COMPRA_ESTOQUE" dataDxfId="22"/>
+    <tableColumn id="4" xr3:uid="{DA9386F6-AAE0-4E57-903A-B2F98B6704B9}" name="DATA" dataDxfId="21"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight10" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{58001711-95ED-4EB3-B06E-017ECCC7FA4B}" name="Tabela7" displayName="Tabela7" ref="A1:F37" totalsRowShown="0" headerRowDxfId="15" dataDxfId="13" headerRowBorderDxfId="14" tableBorderDxfId="12" totalsRowBorderDxfId="11">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{58001711-95ED-4EB3-B06E-017ECCC7FA4B}" name="Tabela7" displayName="Tabela7" ref="A1:F37" totalsRowShown="0" headerRowDxfId="20" dataDxfId="18" headerRowBorderDxfId="19" tableBorderDxfId="17" totalsRowBorderDxfId="16">
   <autoFilter ref="A1:F37" xr:uid="{58001711-95ED-4EB3-B06E-017ECCC7FA4B}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:F37">
     <sortCondition descending="1" ref="D1:D37"/>
   </sortState>
   <tableColumns count="6">
-    <tableColumn id="1" xr3:uid="{FE588C2B-EF40-410F-8547-D20DC2D114DD}" name="ID_PRODUTO" dataDxfId="3"/>
-    <tableColumn id="2" xr3:uid="{4634FBFF-8AC9-49AB-A9DB-3D4D5740D2AE}" name="NOME" dataDxfId="2"/>
-    <tableColumn id="3" xr3:uid="{F5DE94E4-99CE-42D1-AEF4-32E3B71293E2}" name="DESCRICAO" dataDxfId="0"/>
-    <tableColumn id="4" xr3:uid="{1D1D00F6-0C34-4EFE-9CB5-388B09FE6A0F}" name="PRECO" dataDxfId="1"/>
-    <tableColumn id="5" xr3:uid="{09ECF3A4-8519-4D44-944C-22566A11E004}" name="QTD_ESTOQUE" dataDxfId="10"/>
-    <tableColumn id="6" xr3:uid="{A1565A1A-435C-41F9-9AB4-DB585E61FD7D}" name="ID_CATEGORIA" dataDxfId="9"/>
+    <tableColumn id="1" xr3:uid="{FE588C2B-EF40-410F-8547-D20DC2D114DD}" name="ID_PRODUTO" dataDxfId="15"/>
+    <tableColumn id="2" xr3:uid="{4634FBFF-8AC9-49AB-A9DB-3D4D5740D2AE}" name="NOME" dataDxfId="14"/>
+    <tableColumn id="3" xr3:uid="{F5DE94E4-99CE-42D1-AEF4-32E3B71293E2}" name="DESCRICAO" dataDxfId="13"/>
+    <tableColumn id="4" xr3:uid="{1D1D00F6-0C34-4EFE-9CB5-388B09FE6A0F}" name="PRECO" dataDxfId="12"/>
+    <tableColumn id="5" xr3:uid="{09ECF3A4-8519-4D44-944C-22566A11E004}" name="QTD_ESTOQUE" dataDxfId="11"/>
+    <tableColumn id="6" xr3:uid="{A1565A1A-435C-41F9-9AB4-DB585E61FD7D}" name="ID_CATEGORIA" dataDxfId="10"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium17" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -5209,7 +5265,7 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="D2:D100">
-    <cfRule type="duplicateValues" dxfId="8" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="9" priority="1"/>
   </conditionalFormatting>
   <hyperlinks>
     <hyperlink ref="D18" r:id="rId1" xr:uid="{656DED77-40EE-4CDD-947A-8D8BE73C026B}"/>
@@ -5230,10 +5286,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2F2F9615-2D0F-49E8-8681-B8BA1D9C831D}">
-  <dimension ref="A1:E21"/>
+  <dimension ref="A1:E9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E21" sqref="E21"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5246,360 +5302,156 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" s="33" t="s">
+      <c r="A1" s="51" t="s">
         <v>294</v>
       </c>
-      <c r="B1" s="34" t="s">
+      <c r="B1" s="52" t="s">
         <v>295</v>
       </c>
-      <c r="C1" s="34" t="s">
+      <c r="C1" s="52" t="s">
         <v>296</v>
       </c>
-      <c r="D1" s="35" t="s">
+      <c r="D1" s="53" t="s">
         <v>297</v>
       </c>
-      <c r="E1" s="36" t="s">
+      <c r="E1" s="54" t="s">
         <v>88</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" s="4">
-        <v>1</v>
-      </c>
-      <c r="B2" s="11">
-        <v>3399</v>
-      </c>
-      <c r="C2" s="11" t="s">
+      <c r="A2" s="55">
+        <v>30</v>
+      </c>
+      <c r="B2" s="56">
+        <v>9300</v>
+      </c>
+      <c r="C2" s="57" t="s">
         <v>298</v>
       </c>
-      <c r="D2" s="37">
-        <v>44200</v>
-      </c>
-      <c r="E2" s="6">
-        <v>8</v>
+      <c r="D2" s="58">
+        <v>44221</v>
+      </c>
+      <c r="E2" s="59">
+        <v>56</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" s="4">
-        <v>2</v>
-      </c>
-      <c r="B3" s="11">
-        <v>600</v>
-      </c>
-      <c r="C3" s="11" t="s">
+      <c r="A3" s="60">
+        <v>31</v>
+      </c>
+      <c r="B3" s="61">
+        <v>450</v>
+      </c>
+      <c r="C3" s="62" t="s">
         <v>299</v>
       </c>
-      <c r="D3" s="37">
-        <v>44200</v>
-      </c>
-      <c r="E3" s="6">
-        <v>19</v>
+      <c r="D3" s="63">
+        <v>44222</v>
+      </c>
+      <c r="E3" s="64">
+        <v>77</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" s="4">
-        <v>3</v>
-      </c>
-      <c r="B4" s="11">
+      <c r="A4" s="55">
+        <v>32</v>
+      </c>
+      <c r="B4" s="56">
+        <v>430</v>
+      </c>
+      <c r="C4" s="57" t="s">
+        <v>300</v>
+      </c>
+      <c r="D4" s="58">
+        <v>44223</v>
+      </c>
+      <c r="E4" s="59">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" s="60">
+        <v>33</v>
+      </c>
+      <c r="B5" s="61">
+        <v>700</v>
+      </c>
+      <c r="C5" s="62" t="s">
+        <v>299</v>
+      </c>
+      <c r="D5" s="63">
+        <v>44224</v>
+      </c>
+      <c r="E5" s="64">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" s="55">
+        <v>34</v>
+      </c>
+      <c r="B6" s="56">
+        <v>150</v>
+      </c>
+      <c r="C6" s="57" t="s">
+        <v>300</v>
+      </c>
+      <c r="D6" s="58">
+        <v>44225</v>
+      </c>
+      <c r="E6" s="59">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" s="60">
+        <v>35</v>
+      </c>
+      <c r="B7" s="61">
         <v>100</v>
       </c>
-      <c r="C4" s="11" t="s">
+      <c r="C7" s="62" t="s">
         <v>300</v>
       </c>
-      <c r="D4" s="37">
-        <v>44201</v>
-      </c>
-      <c r="E4" s="6">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" s="4">
-        <v>4</v>
-      </c>
-      <c r="B5" s="11">
-        <v>200</v>
-      </c>
-      <c r="C5" s="11" t="s">
-        <v>300</v>
-      </c>
-      <c r="D5" s="37">
-        <v>44201</v>
-      </c>
-      <c r="E5" s="6">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" s="4">
-        <v>5</v>
-      </c>
-      <c r="B6" s="11">
-        <v>150</v>
-      </c>
-      <c r="C6" s="11" t="s">
+      <c r="D7" s="63">
+        <v>44225</v>
+      </c>
+      <c r="E7" s="64">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" s="55">
+        <v>36</v>
+      </c>
+      <c r="B8" s="56">
+        <v>100</v>
+      </c>
+      <c r="C8" s="57" t="s">
         <v>299</v>
       </c>
-      <c r="D6" s="37">
-        <v>44201</v>
-      </c>
-      <c r="E6" s="6">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" s="4">
-        <v>6</v>
-      </c>
-      <c r="B7" s="11">
-        <v>250</v>
-      </c>
-      <c r="C7" s="11" t="s">
+      <c r="D8" s="58">
+        <v>44225</v>
+      </c>
+      <c r="E8" s="59">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" s="65">
+        <v>37</v>
+      </c>
+      <c r="B9" s="66">
+        <v>100</v>
+      </c>
+      <c r="C9" s="67" t="s">
         <v>299</v>
       </c>
-      <c r="D7" s="37">
-        <v>44202</v>
-      </c>
-      <c r="E7" s="6">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8" s="7">
-        <v>7</v>
-      </c>
-      <c r="B8" s="12">
-        <v>500</v>
-      </c>
-      <c r="C8" s="12" t="s">
-        <v>299</v>
-      </c>
-      <c r="D8" s="38">
-        <v>44202</v>
-      </c>
-      <c r="E8" s="9">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A9" s="7">
-        <v>8</v>
-      </c>
-      <c r="B9" s="12">
-        <v>200</v>
-      </c>
-      <c r="C9" s="12" t="s">
-        <v>301</v>
-      </c>
-      <c r="D9" s="38">
-        <v>44202</v>
-      </c>
-      <c r="E9" s="9">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A10" s="7">
-        <v>9</v>
-      </c>
-      <c r="B10" s="12">
-        <v>600</v>
-      </c>
-      <c r="C10" s="12" t="s">
-        <v>301</v>
-      </c>
-      <c r="D10" s="38">
-        <v>44202</v>
-      </c>
-      <c r="E10" s="9">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A11" s="7">
-        <v>10</v>
-      </c>
-      <c r="B11" s="12">
-        <v>1600</v>
-      </c>
-      <c r="C11" s="12" t="s">
-        <v>298</v>
-      </c>
-      <c r="D11" s="38">
-        <v>44203</v>
-      </c>
-      <c r="E11" s="9">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A12" s="7">
+      <c r="D9" s="68">
+        <v>44225</v>
+      </c>
+      <c r="E9" s="69">
         <v>11</v>
-      </c>
-      <c r="B12" s="12">
-        <v>150</v>
-      </c>
-      <c r="C12" s="12" t="s">
-        <v>300</v>
-      </c>
-      <c r="D12" s="38">
-        <v>44204</v>
-      </c>
-      <c r="E12" s="9">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A13" s="7">
-        <v>12</v>
-      </c>
-      <c r="B13" s="12">
-        <v>4200</v>
-      </c>
-      <c r="C13" s="12" t="s">
-        <v>298</v>
-      </c>
-      <c r="D13" s="38">
-        <v>44207</v>
-      </c>
-      <c r="E13" s="9">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A14" s="7">
-        <v>13</v>
-      </c>
-      <c r="B14" s="12">
-        <v>500</v>
-      </c>
-      <c r="C14" s="12" t="s">
-        <v>299</v>
-      </c>
-      <c r="D14" s="38">
-        <v>44207</v>
-      </c>
-      <c r="E14" s="9">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A15" s="7">
-        <v>14</v>
-      </c>
-      <c r="B15" s="12">
-        <v>180</v>
-      </c>
-      <c r="C15" s="12" t="s">
-        <v>299</v>
-      </c>
-      <c r="D15" s="38">
-        <v>44207</v>
-      </c>
-      <c r="E15" s="9">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A16" s="7">
-        <v>15</v>
-      </c>
-      <c r="B16" s="12">
-        <v>50</v>
-      </c>
-      <c r="C16" s="12" t="s">
-        <v>300</v>
-      </c>
-      <c r="D16" s="38">
-        <v>44208</v>
-      </c>
-      <c r="E16" s="9">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A17" s="7">
-        <v>16</v>
-      </c>
-      <c r="B17" s="12">
-        <v>100</v>
-      </c>
-      <c r="C17" s="12" t="s">
-        <v>299</v>
-      </c>
-      <c r="D17" s="38">
-        <v>44209</v>
-      </c>
-      <c r="E17" s="9">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A18" s="7">
-        <v>17</v>
-      </c>
-      <c r="B18" s="12">
-        <v>200</v>
-      </c>
-      <c r="C18" s="12" t="s">
-        <v>301</v>
-      </c>
-      <c r="D18" s="38">
-        <v>44209</v>
-      </c>
-      <c r="E18" s="9">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A19" s="7">
-        <v>18</v>
-      </c>
-      <c r="B19" s="12">
-        <v>250</v>
-      </c>
-      <c r="C19" s="12" t="s">
-        <v>298</v>
-      </c>
-      <c r="D19" s="38">
-        <v>44209</v>
-      </c>
-      <c r="E19" s="9">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A20" s="7">
-        <v>19</v>
-      </c>
-      <c r="B20" s="12">
-        <v>1280</v>
-      </c>
-      <c r="C20" s="12" t="s">
-        <v>301</v>
-      </c>
-      <c r="D20" s="38">
-        <v>44210</v>
-      </c>
-      <c r="E20" s="9">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A21" s="7">
-        <v>20</v>
-      </c>
-      <c r="B21" s="12">
-        <v>980</v>
-      </c>
-      <c r="C21" s="12" t="s">
-        <v>298</v>
-      </c>
-      <c r="D21" s="38">
-        <v>44211</v>
-      </c>
-      <c r="E21" s="9">
-        <v>71</v>
       </c>
     </row>
   </sheetData>
@@ -5614,34 +5466,34 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D8E37E1D-E48D-467F-9C97-1887D965FB08}">
   <dimension ref="A1:E31"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A29" sqref="A29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="18" style="40" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.42578125" style="40" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15" style="40" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.42578125" style="40" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="20.7109375" style="41" customWidth="1"/>
+    <col min="1" max="1" width="18" style="34" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.42578125" style="34" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15" style="34" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.42578125" style="34" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="20.7109375" style="35" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
+        <v>301</v>
+      </c>
+      <c r="B1" s="2" t="s">
         <v>302</v>
-      </c>
-      <c r="B1" s="2" t="s">
-        <v>303</v>
       </c>
       <c r="C1" s="2" t="s">
         <v>66</v>
       </c>
       <c r="D1" s="2" t="s">
+        <v>303</v>
+      </c>
+      <c r="E1" s="10" t="s">
         <v>304</v>
-      </c>
-      <c r="E1" s="10" t="s">
-        <v>305</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
@@ -6141,7 +5993,7 @@
       <c r="A31" s="7">
         <v>30</v>
       </c>
-      <c r="B31" s="39">
+      <c r="B31" s="33">
         <v>20</v>
       </c>
       <c r="C31" s="8">
@@ -6997,7 +6849,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{75023552-0E84-4DB2-9D27-8ACF572B4AA1}">
   <dimension ref="A1:F37"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
@@ -7012,755 +6864,746 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" s="46" t="s">
+      <c r="A1" s="40" t="s">
         <v>66</v>
       </c>
-      <c r="B1" s="47" t="s">
+      <c r="B1" s="41" t="s">
         <v>67</v>
       </c>
-      <c r="C1" s="47" t="s">
+      <c r="C1" s="41" t="s">
         <v>68</v>
       </c>
-      <c r="D1" s="48" t="s">
+      <c r="D1" s="42" t="s">
         <v>69</v>
       </c>
-      <c r="E1" s="47" t="s">
+      <c r="E1" s="41" t="s">
         <v>70</v>
       </c>
-      <c r="F1" s="49" t="s">
+      <c r="F1" s="43" t="s">
         <v>71</v>
       </c>
     </row>
     <row r="2" spans="1:6" ht="15.75" x14ac:dyDescent="0.3">
-      <c r="A2" s="44">
+      <c r="A2" s="38">
         <v>5</v>
       </c>
-      <c r="B2" s="54" t="s">
+      <c r="B2" s="48" t="s">
         <v>6</v>
       </c>
-      <c r="C2" s="54" t="s">
+      <c r="C2" s="48" t="s">
         <v>5</v>
       </c>
-      <c r="D2" s="43">
+      <c r="D2" s="37">
         <v>4200</v>
       </c>
-      <c r="E2" s="42">
+      <c r="E2" s="36">
         <v>1</v>
       </c>
-      <c r="F2" s="45">
+      <c r="F2" s="39">
         <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="15.75" x14ac:dyDescent="0.3">
-      <c r="A3" s="44">
+      <c r="A3" s="38">
         <v>3</v>
       </c>
-      <c r="B3" s="54" t="s">
+      <c r="B3" s="48" t="s">
         <v>3</v>
       </c>
-      <c r="C3" s="54" t="s">
+      <c r="C3" s="48" t="s">
         <v>1</v>
       </c>
-      <c r="D3" s="43">
+      <c r="D3" s="37">
         <v>3900</v>
       </c>
-      <c r="E3" s="42">
+      <c r="E3" s="36">
         <v>3</v>
       </c>
-      <c r="F3" s="45">
+      <c r="F3" s="39">
         <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="15.75" x14ac:dyDescent="0.3">
-      <c r="A4" s="44">
+      <c r="A4" s="38">
         <v>2</v>
       </c>
-      <c r="B4" s="54" t="s">
-        <v>306</v>
-      </c>
-      <c r="C4" s="54" t="s">
+      <c r="B4" s="48" t="s">
+        <v>305</v>
+      </c>
+      <c r="C4" s="48" t="s">
         <v>1</v>
       </c>
-      <c r="D4" s="43">
+      <c r="D4" s="37">
         <v>3500</v>
       </c>
-      <c r="E4" s="42">
+      <c r="E4" s="36">
         <v>4</v>
       </c>
-      <c r="F4" s="45">
+      <c r="F4" s="39">
         <v>1</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="15.75" x14ac:dyDescent="0.3">
-      <c r="A5" s="44">
+      <c r="A5" s="38">
         <v>1</v>
       </c>
-      <c r="B5" s="54" t="s">
+      <c r="B5" s="48" t="s">
         <v>0</v>
       </c>
-      <c r="C5" s="54" t="s">
+      <c r="C5" s="48" t="s">
         <v>1</v>
       </c>
-      <c r="D5" s="43">
+      <c r="D5" s="37">
         <v>3200</v>
       </c>
-      <c r="E5" s="42">
+      <c r="E5" s="36">
         <v>4</v>
       </c>
-      <c r="F5" s="45">
+      <c r="F5" s="39">
         <v>1</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="15.75" x14ac:dyDescent="0.3">
-      <c r="A6" s="44">
+      <c r="A6" s="38">
         <v>4</v>
       </c>
-      <c r="B6" s="54" t="s">
+      <c r="B6" s="48" t="s">
         <v>4</v>
       </c>
-      <c r="C6" s="54" t="s">
+      <c r="C6" s="48" t="s">
         <v>5</v>
       </c>
-      <c r="D6" s="43">
+      <c r="D6" s="37">
         <v>2600</v>
       </c>
-      <c r="E6" s="42">
+      <c r="E6" s="36">
         <v>4</v>
       </c>
-      <c r="F6" s="56">
+      <c r="F6" s="50">
         <v>1</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="15.75" x14ac:dyDescent="0.3">
-      <c r="A7" s="44">
+      <c r="A7" s="38">
         <v>18</v>
       </c>
-      <c r="B7" s="54" t="s">
+      <c r="B7" s="48" t="s">
         <v>28</v>
       </c>
-      <c r="C7" s="54" t="s">
+      <c r="C7" s="48" t="s">
         <v>29</v>
       </c>
-      <c r="D7" s="43">
+      <c r="D7" s="37">
         <v>1200</v>
       </c>
-      <c r="E7" s="42">
+      <c r="E7" s="36">
         <v>3</v>
       </c>
-      <c r="F7" s="45">
+      <c r="F7" s="39">
         <v>15</v>
       </c>
     </row>
     <row r="8" spans="1:6" ht="15.75" x14ac:dyDescent="0.3">
-      <c r="A8" s="44">
+      <c r="A8" s="38">
         <v>35</v>
       </c>
-      <c r="B8" s="54" t="s">
+      <c r="B8" s="48" t="s">
         <v>62</v>
       </c>
-      <c r="C8" s="54" t="s">
+      <c r="C8" s="48" t="s">
         <v>63</v>
       </c>
-      <c r="D8" s="43">
+      <c r="D8" s="37">
         <v>500</v>
       </c>
-      <c r="E8" s="42">
+      <c r="E8" s="36">
         <v>1</v>
       </c>
-      <c r="F8" s="45">
+      <c r="F8" s="39">
         <v>17</v>
       </c>
     </row>
     <row r="9" spans="1:6" ht="15.75" x14ac:dyDescent="0.3">
-      <c r="A9" s="44">
+      <c r="A9" s="38">
         <v>6</v>
       </c>
-      <c r="B9" s="54" t="s">
+      <c r="B9" s="48" t="s">
         <v>7</v>
       </c>
-      <c r="C9" s="54" t="s">
+      <c r="C9" s="48" t="s">
         <v>7</v>
       </c>
-      <c r="D9" s="43">
+      <c r="D9" s="37">
         <v>430</v>
       </c>
-      <c r="E9" s="42">
+      <c r="E9" s="36">
         <v>5</v>
       </c>
-      <c r="F9" s="45">
+      <c r="F9" s="39">
         <v>9</v>
       </c>
     </row>
     <row r="10" spans="1:6" ht="15.75" x14ac:dyDescent="0.3">
-      <c r="A10" s="44">
+      <c r="A10" s="38">
         <v>7</v>
       </c>
-      <c r="B10" s="54" t="s">
+      <c r="B10" s="48" t="s">
         <v>8</v>
       </c>
-      <c r="C10" s="54" t="s">
+      <c r="C10" s="48" t="s">
         <v>8</v>
       </c>
-      <c r="D10" s="43">
+      <c r="D10" s="37">
         <v>430</v>
       </c>
-      <c r="E10" s="42">
+      <c r="E10" s="36">
         <v>3</v>
       </c>
-      <c r="F10" s="45">
+      <c r="F10" s="39">
         <v>10</v>
       </c>
     </row>
     <row r="11" spans="1:6" ht="15.75" x14ac:dyDescent="0.3">
-      <c r="A11" s="44">
+      <c r="A11" s="38">
         <v>25</v>
       </c>
-      <c r="B11" s="54" t="s">
+      <c r="B11" s="48" t="s">
         <v>42</v>
       </c>
-      <c r="C11" s="54" t="s">
+      <c r="C11" s="48" t="s">
         <v>43</v>
       </c>
-      <c r="D11" s="43">
+      <c r="D11" s="37">
         <v>400</v>
       </c>
-      <c r="E11" s="42">
+      <c r="E11" s="36">
         <v>6</v>
       </c>
-      <c r="F11" s="45">
+      <c r="F11" s="39">
         <v>7</v>
       </c>
     </row>
     <row r="12" spans="1:6" ht="15.75" x14ac:dyDescent="0.3">
-      <c r="A12" s="44">
+      <c r="A12" s="38">
         <v>33</v>
       </c>
-      <c r="B12" s="54" t="s">
+      <c r="B12" s="48" t="s">
         <v>58</v>
       </c>
-      <c r="C12" s="54" t="s">
+      <c r="C12" s="48" t="s">
         <v>59</v>
       </c>
-      <c r="D12" s="43">
+      <c r="D12" s="37">
         <v>400</v>
       </c>
-      <c r="E12" s="42">
+      <c r="E12" s="36">
         <v>4</v>
       </c>
-      <c r="F12" s="45">
+      <c r="F12" s="39">
         <v>11</v>
       </c>
     </row>
     <row r="13" spans="1:6" ht="15.75" x14ac:dyDescent="0.3">
-      <c r="A13" s="44">
+      <c r="A13" s="38">
         <v>11</v>
       </c>
-      <c r="B13" s="54" t="s">
+      <c r="B13" s="48" t="s">
         <v>14</v>
       </c>
-      <c r="C13" s="54" t="s">
+      <c r="C13" s="48" t="s">
         <v>15</v>
       </c>
-      <c r="D13" s="43">
+      <c r="D13" s="37">
         <v>350</v>
       </c>
-      <c r="E13" s="42">
+      <c r="E13" s="36">
         <v>9</v>
       </c>
-      <c r="F13" s="45">
+      <c r="F13" s="39">
         <v>11</v>
       </c>
     </row>
     <row r="14" spans="1:6" ht="15.75" x14ac:dyDescent="0.3">
-      <c r="A14" s="44">
+      <c r="A14" s="38">
         <v>19</v>
       </c>
-      <c r="B14" s="54" t="s">
+      <c r="B14" s="48" t="s">
         <v>30</v>
       </c>
-      <c r="C14" s="54" t="s">
+      <c r="C14" s="48" t="s">
         <v>31</v>
       </c>
-      <c r="D14" s="43">
+      <c r="D14" s="37">
         <v>350</v>
       </c>
-      <c r="E14" s="42">
+      <c r="E14" s="36">
         <v>6</v>
       </c>
-      <c r="F14" s="45">
+      <c r="F14" s="39">
         <v>16</v>
       </c>
     </row>
     <row r="15" spans="1:6" ht="15.75" x14ac:dyDescent="0.3">
-      <c r="A15" s="44">
+      <c r="A15" s="38">
         <v>20</v>
       </c>
-      <c r="B15" s="54" t="s">
+      <c r="B15" s="48" t="s">
         <v>32</v>
       </c>
-      <c r="C15" s="54" t="s">
+      <c r="C15" s="48" t="s">
         <v>33</v>
       </c>
-      <c r="D15" s="43">
+      <c r="D15" s="37">
         <v>350</v>
       </c>
-      <c r="E15" s="42">
+      <c r="E15" s="36">
         <v>3</v>
       </c>
-      <c r="F15" s="45">
+      <c r="F15" s="39">
         <v>16</v>
       </c>
     </row>
     <row r="16" spans="1:6" ht="15.75" x14ac:dyDescent="0.3">
-      <c r="A16" s="44">
+      <c r="A16" s="38">
         <v>15</v>
       </c>
-      <c r="B16" s="54" t="s">
+      <c r="B16" s="48" t="s">
         <v>22</v>
       </c>
-      <c r="C16" s="54" t="s">
+      <c r="C16" s="48" t="s">
         <v>23</v>
       </c>
-      <c r="D16" s="43">
+      <c r="D16" s="37">
         <v>300</v>
       </c>
-      <c r="E16" s="42">
+      <c r="E16" s="36">
         <v>8</v>
       </c>
-      <c r="F16" s="45">
+      <c r="F16" s="39">
         <v>3</v>
       </c>
     </row>
     <row r="17" spans="1:6" ht="15.75" x14ac:dyDescent="0.3">
-      <c r="A17" s="44">
+      <c r="A17" s="38">
         <v>22</v>
       </c>
-      <c r="B17" s="54" t="s">
+      <c r="B17" s="48" t="s">
         <v>36</v>
       </c>
-      <c r="C17" s="54" t="s">
+      <c r="C17" s="48" t="s">
         <v>37</v>
       </c>
-      <c r="D17" s="43">
+      <c r="D17" s="37">
         <v>300</v>
       </c>
-      <c r="E17" s="42">
+      <c r="E17" s="36">
         <v>4</v>
       </c>
-      <c r="F17" s="45">
+      <c r="F17" s="39">
         <v>3</v>
       </c>
     </row>
     <row r="18" spans="1:6" ht="15.75" x14ac:dyDescent="0.3">
-      <c r="A18" s="44">
+      <c r="A18" s="38">
         <v>24</v>
       </c>
-      <c r="B18" s="54" t="s">
+      <c r="B18" s="48" t="s">
         <v>40</v>
       </c>
-      <c r="C18" s="54" t="s">
+      <c r="C18" s="48" t="s">
         <v>41</v>
       </c>
-      <c r="D18" s="43">
+      <c r="D18" s="37">
         <v>300</v>
       </c>
-      <c r="E18" s="42">
+      <c r="E18" s="36">
         <v>3</v>
       </c>
-      <c r="F18" s="45">
+      <c r="F18" s="39">
         <v>5</v>
       </c>
     </row>
     <row r="19" spans="1:6" ht="15.75" x14ac:dyDescent="0.3">
-      <c r="A19" s="44">
+      <c r="A19" s="38">
         <v>27</v>
       </c>
-      <c r="B19" s="54" t="s">
+      <c r="B19" s="48" t="s">
         <v>46</v>
       </c>
-      <c r="C19" s="54" t="s">
+      <c r="C19" s="48" t="s">
         <v>47</v>
       </c>
-      <c r="D19" s="43">
+      <c r="D19" s="37">
         <v>300</v>
       </c>
-      <c r="E19" s="42">
+      <c r="E19" s="36">
         <v>4</v>
       </c>
-      <c r="F19" s="45">
+      <c r="F19" s="39">
         <v>2</v>
       </c>
     </row>
     <row r="20" spans="1:6" ht="15.75" x14ac:dyDescent="0.3">
-      <c r="A20" s="44">
+      <c r="A20" s="38">
         <v>29</v>
       </c>
-      <c r="B20" s="54" t="s">
+      <c r="B20" s="48" t="s">
         <v>50</v>
       </c>
-      <c r="C20" s="54" t="s">
+      <c r="C20" s="48" t="s">
         <v>51</v>
       </c>
-      <c r="D20" s="43">
+      <c r="D20" s="37">
         <v>300</v>
       </c>
-      <c r="E20" s="42">
+      <c r="E20" s="36">
         <v>9</v>
       </c>
-      <c r="F20" s="45">
+      <c r="F20" s="39">
         <v>6</v>
       </c>
     </row>
     <row r="21" spans="1:6" ht="15.75" x14ac:dyDescent="0.3">
-      <c r="A21" s="44">
+      <c r="A21" s="38">
         <v>32</v>
       </c>
-      <c r="B21" s="54" t="s">
+      <c r="B21" s="48" t="s">
         <v>56</v>
       </c>
-      <c r="C21" s="54" t="s">
+      <c r="C21" s="48" t="s">
         <v>57</v>
       </c>
-      <c r="D21" s="43">
+      <c r="D21" s="37">
         <v>300</v>
       </c>
-      <c r="E21" s="42">
+      <c r="E21" s="36">
         <v>5</v>
       </c>
-      <c r="F21" s="45">
+      <c r="F21" s="39">
         <v>5</v>
       </c>
     </row>
     <row r="22" spans="1:6" ht="15.75" x14ac:dyDescent="0.3">
-      <c r="A22" s="44">
+      <c r="A22" s="38">
         <v>10</v>
       </c>
-      <c r="B22" s="54" t="s">
+      <c r="B22" s="48" t="s">
         <v>12</v>
       </c>
-      <c r="C22" s="54" t="s">
+      <c r="C22" s="48" t="s">
         <v>13</v>
       </c>
-      <c r="D22" s="43">
+      <c r="D22" s="37">
         <v>250</v>
       </c>
-      <c r="E22" s="42">
+      <c r="E22" s="36">
         <v>13</v>
       </c>
-      <c r="F22" s="45">
+      <c r="F22" s="39">
         <v>6</v>
       </c>
     </row>
     <row r="23" spans="1:6" ht="15.75" x14ac:dyDescent="0.3">
-      <c r="A23" s="44">
+      <c r="A23" s="38">
         <v>16</v>
       </c>
-      <c r="B23" s="54" t="s">
+      <c r="B23" s="48" t="s">
         <v>24</v>
       </c>
-      <c r="C23" s="54" t="s">
+      <c r="C23" s="48" t="s">
         <v>25</v>
       </c>
-      <c r="D23" s="43">
+      <c r="D23" s="37">
         <v>250</v>
       </c>
-      <c r="E23" s="42">
+      <c r="E23" s="36">
         <v>4</v>
       </c>
-      <c r="F23" s="45">
+      <c r="F23" s="39">
         <v>4</v>
       </c>
     </row>
     <row r="24" spans="1:6" ht="15.75" x14ac:dyDescent="0.3">
-      <c r="A24" s="44">
+      <c r="A24" s="38">
         <v>21</v>
       </c>
-      <c r="B24" s="54" t="s">
+      <c r="B24" s="48" t="s">
         <v>34</v>
       </c>
-      <c r="C24" s="54" t="s">
+      <c r="C24" s="48" t="s">
         <v>35</v>
       </c>
-      <c r="D24" s="43">
+      <c r="D24" s="37">
         <v>250</v>
       </c>
-      <c r="E24" s="42">
+      <c r="E24" s="36">
         <v>5</v>
       </c>
-      <c r="F24" s="45">
+      <c r="F24" s="39">
         <v>3</v>
       </c>
     </row>
     <row r="25" spans="1:6" ht="15.75" x14ac:dyDescent="0.3">
-      <c r="A25" s="44">
+      <c r="A25" s="38">
         <v>23</v>
       </c>
-      <c r="B25" s="54" t="s">
+      <c r="B25" s="48" t="s">
         <v>38</v>
       </c>
-      <c r="C25" s="54" t="s">
+      <c r="C25" s="48" t="s">
         <v>39</v>
       </c>
-      <c r="D25" s="43">
+      <c r="D25" s="37">
         <v>250</v>
       </c>
-      <c r="E25" s="42">
+      <c r="E25" s="36">
         <v>6</v>
       </c>
-      <c r="F25" s="45">
+      <c r="F25" s="39">
         <v>16</v>
       </c>
     </row>
     <row r="26" spans="1:6" ht="15.75" x14ac:dyDescent="0.3">
-      <c r="A26" s="44">
+      <c r="A26" s="38">
         <v>31</v>
       </c>
-      <c r="B26" s="54" t="s">
+      <c r="B26" s="48" t="s">
         <v>54</v>
       </c>
-      <c r="C26" s="54" t="s">
+      <c r="C26" s="48" t="s">
         <v>55</v>
       </c>
-      <c r="D26" s="43">
+      <c r="D26" s="37">
         <v>250</v>
       </c>
-      <c r="E26" s="42">
+      <c r="E26" s="36">
         <v>6</v>
       </c>
-      <c r="F26" s="45">
+      <c r="F26" s="39">
         <v>3</v>
       </c>
     </row>
     <row r="27" spans="1:6" ht="15.75" x14ac:dyDescent="0.3">
-      <c r="A27" s="44">
+      <c r="A27" s="38">
         <v>13</v>
       </c>
-      <c r="B27" s="54" t="s">
+      <c r="B27" s="48" t="s">
         <v>18</v>
       </c>
-      <c r="C27" s="54" t="s">
+      <c r="C27" s="48" t="s">
         <v>19</v>
       </c>
-      <c r="D27" s="43">
+      <c r="D27" s="37">
         <v>200</v>
       </c>
-      <c r="E27" s="42">
+      <c r="E27" s="36">
         <v>10</v>
       </c>
-      <c r="F27" s="45">
+      <c r="F27" s="39">
         <v>13</v>
       </c>
     </row>
     <row r="28" spans="1:6" ht="15.75" x14ac:dyDescent="0.3">
-      <c r="A28" s="44">
+      <c r="A28" s="38">
         <v>14</v>
       </c>
-      <c r="B28" s="54" t="s">
+      <c r="B28" s="48" t="s">
         <v>20</v>
       </c>
-      <c r="C28" s="54" t="s">
+      <c r="C28" s="48" t="s">
         <v>21</v>
       </c>
-      <c r="D28" s="43">
+      <c r="D28" s="37">
         <v>200</v>
       </c>
-      <c r="E28" s="42">
+      <c r="E28" s="36">
         <v>8</v>
       </c>
-      <c r="F28" s="45">
+      <c r="F28" s="39">
         <v>14</v>
       </c>
     </row>
     <row r="29" spans="1:6" ht="15.75" x14ac:dyDescent="0.3">
-      <c r="A29" s="44">
+      <c r="A29" s="38">
         <v>28</v>
       </c>
-      <c r="B29" s="54" t="s">
+      <c r="B29" s="48" t="s">
         <v>48</v>
       </c>
-      <c r="C29" s="54" t="s">
+      <c r="C29" s="48" t="s">
         <v>49</v>
       </c>
-      <c r="D29" s="43">
+      <c r="D29" s="37">
         <v>200</v>
       </c>
-      <c r="E29" s="42">
+      <c r="E29" s="36">
         <v>4</v>
       </c>
-      <c r="F29" s="45">
+      <c r="F29" s="39">
         <v>2</v>
       </c>
     </row>
     <row r="30" spans="1:6" ht="15.75" x14ac:dyDescent="0.3">
-      <c r="A30" s="44">
+      <c r="A30" s="38">
         <v>34</v>
       </c>
-      <c r="B30" s="54" t="s">
+      <c r="B30" s="48" t="s">
         <v>60</v>
       </c>
-      <c r="C30" s="54" t="s">
+      <c r="C30" s="48" t="s">
         <v>61</v>
       </c>
-      <c r="D30" s="43">
+      <c r="D30" s="37">
         <v>200</v>
       </c>
-      <c r="E30" s="42">
+      <c r="E30" s="36">
         <v>9</v>
       </c>
-      <c r="F30" s="45">
+      <c r="F30" s="39">
         <v>12</v>
       </c>
     </row>
     <row r="31" spans="1:6" ht="15.75" x14ac:dyDescent="0.3">
-      <c r="A31" s="44">
+      <c r="A31" s="38">
         <v>12</v>
       </c>
-      <c r="B31" s="54" t="s">
+      <c r="B31" s="48" t="s">
         <v>16</v>
       </c>
-      <c r="C31" s="54" t="s">
+      <c r="C31" s="48" t="s">
         <v>17</v>
       </c>
-      <c r="D31" s="43">
+      <c r="D31" s="37">
         <v>180</v>
       </c>
-      <c r="E31" s="42">
+      <c r="E31" s="36">
         <v>10</v>
       </c>
-      <c r="F31" s="45">
+      <c r="F31" s="39">
         <v>12</v>
       </c>
     </row>
     <row r="32" spans="1:6" ht="15.75" x14ac:dyDescent="0.3">
-      <c r="A32" s="44">
+      <c r="A32" s="38">
         <v>17</v>
       </c>
-      <c r="B32" s="54" t="s">
+      <c r="B32" s="48" t="s">
         <v>26</v>
       </c>
-      <c r="C32" s="54" t="s">
+      <c r="C32" s="48" t="s">
         <v>27</v>
       </c>
-      <c r="D32" s="43">
+      <c r="D32" s="37">
         <v>150</v>
       </c>
-      <c r="E32" s="42">
+      <c r="E32" s="36">
         <v>6</v>
       </c>
-      <c r="F32" s="45">
+      <c r="F32" s="39">
         <v>2</v>
       </c>
     </row>
     <row r="33" spans="1:6" ht="15.75" x14ac:dyDescent="0.3">
-      <c r="A33" s="44">
+      <c r="A33" s="38">
         <v>36</v>
       </c>
-      <c r="B33" s="54" t="s">
+      <c r="B33" s="48" t="s">
         <v>64</v>
       </c>
-      <c r="C33" s="54" t="s">
+      <c r="C33" s="48" t="s">
         <v>65</v>
       </c>
-      <c r="D33" s="43">
+      <c r="D33" s="37">
         <v>150</v>
       </c>
-      <c r="E33" s="42">
+      <c r="E33" s="36">
         <v>9</v>
       </c>
-      <c r="F33" s="45">
+      <c r="F33" s="39">
         <v>17</v>
       </c>
     </row>
     <row r="34" spans="1:6" ht="15.75" x14ac:dyDescent="0.3">
-      <c r="A34" s="44">
+      <c r="A34" s="38">
         <v>8</v>
       </c>
-      <c r="B34" s="54" t="s">
+      <c r="B34" s="48" t="s">
         <v>9</v>
       </c>
-      <c r="C34" s="54" t="s">
+      <c r="C34" s="48" t="s">
         <v>10</v>
       </c>
-      <c r="D34" s="43">
+      <c r="D34" s="37">
         <v>100</v>
       </c>
-      <c r="E34" s="42">
+      <c r="E34" s="36">
         <v>18</v>
       </c>
-      <c r="F34" s="45">
+      <c r="F34" s="39">
         <v>13</v>
       </c>
     </row>
     <row r="35" spans="1:6" ht="15.75" x14ac:dyDescent="0.3">
-      <c r="A35" s="44">
+      <c r="A35" s="38">
         <v>9</v>
       </c>
-      <c r="B35" s="54" t="s">
+      <c r="B35" s="48" t="s">
         <v>11</v>
       </c>
-      <c r="C35" s="54" t="s">
+      <c r="C35" s="48" t="s">
         <v>10</v>
       </c>
-      <c r="D35" s="43">
+      <c r="D35" s="37">
         <v>100</v>
       </c>
-      <c r="E35" s="42">
+      <c r="E35" s="36">
         <v>19</v>
       </c>
-      <c r="F35" s="45">
+      <c r="F35" s="39">
         <v>14</v>
       </c>
     </row>
     <row r="36" spans="1:6" ht="15.75" x14ac:dyDescent="0.3">
-      <c r="A36" s="44">
+      <c r="A36" s="38">
         <v>26</v>
       </c>
-      <c r="B36" s="54" t="s">
+      <c r="B36" s="48" t="s">
         <v>44</v>
       </c>
-      <c r="C36" s="54" t="s">
+      <c r="C36" s="48" t="s">
         <v>45</v>
       </c>
-      <c r="D36" s="43">
+      <c r="D36" s="37">
         <v>100</v>
       </c>
-      <c r="E36" s="42">
+      <c r="E36" s="36">
         <v>11</v>
       </c>
-      <c r="F36" s="45">
+      <c r="F36" s="39">
         <v>18</v>
       </c>
     </row>
     <row r="37" spans="1:6" ht="15.75" x14ac:dyDescent="0.3">
-      <c r="A37" s="50">
+      <c r="A37" s="44">
         <v>30</v>
       </c>
-      <c r="B37" s="55" t="s">
+      <c r="B37" s="49" t="s">
         <v>52</v>
       </c>
-      <c r="C37" s="55" t="s">
+      <c r="C37" s="49" t="s">
         <v>53</v>
       </c>
-      <c r="D37" s="52">
+      <c r="D37" s="46">
         <v>50</v>
       </c>
-      <c r="E37" s="51">
+      <c r="E37" s="45">
         <v>19</v>
       </c>
-      <c r="F37" s="53">
+      <c r="F37" s="47">
         <v>17</v>
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="E2:E37">
-    <cfRule type="cellIs" dxfId="7" priority="2" operator="between">
-      <formula>4</formula>
-      <formula>8</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="6" priority="3" operator="lessThan">
-      <formula>3</formula>
-    </cfRule>
-  </conditionalFormatting>
   <conditionalFormatting sqref="D2:D37">
     <cfRule type="dataBar" priority="1">
       <dataBar>
@@ -7773,6 +7616,15 @@
           <x14:id>{E9DEA386-8761-4B96-B490-D1C48EA64D4D}</x14:id>
         </ext>
       </extLst>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E2:E37">
+    <cfRule type="cellIs" dxfId="8" priority="2" operator="between">
+      <formula>4</formula>
+      <formula>8</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="7" priority="3" operator="lessThan">
+      <formula>3</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>

</xml_diff>